<commit_message>
Update Overflow and Underflow statuses 1. Update the code to have  a status word.  Layout started to be defined. 2. Include Variables for calculations which would not require multiple clock cycles for add/sub and setting status word. 3. Clean up other operations to use the variables.  Makes the code a little less wordy. 4. Changed the Immediate ALU operations to set R1 with the R2 and Immediate.  Example R1 = R2 + Imm. 4. Tested in hardware. Not Completed. 1. How to handle the status word.  Gussing needing a new operations to get the status word and clear status word. 2. Thinking about one interrupt for when the status word changes.  Mask to select the changed status words.  Operation to set the mask. 3. Combine the status word and the IO Status into one word.
</commit_message>
<xml_diff>
--- a/ALUOpcodeChanges.xlsx
+++ b/ALUOpcodeChanges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Craig\Documents\000_ArtyS7\CPU2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F5514A-DA57-4DE4-AE16-6A352E277521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA66976-D532-4AB2-AC43-CE2FC81000B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1C340868-20E9-4856-BC56-A25E64F34E4A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="70">
   <si>
     <t>Command</t>
   </si>
@@ -265,7 +265,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,12 +275,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -297,13 +291,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,7 +614,7 @@
   <dimension ref="A2:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F3" sqref="F3:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,16 +686,16 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
@@ -725,7 +718,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="F4" t="s">
@@ -742,6 +735,21 @@
       </c>
       <c r="J4" t="s">
         <v>66</v>
+      </c>
+      <c r="K4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -760,16 +768,16 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5">
         <v>3</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" t="s">
@@ -792,7 +800,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="F6" t="s">
@@ -809,6 +817,21 @@
       </c>
       <c r="J6" t="s">
         <v>66</v>
+      </c>
+      <c r="K6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>